<commit_message>
Temp rename dataNexusDataLake -> temp_DataNexusDataLake
</commit_message>
<xml_diff>
--- a/testData/Driver_Sanity.xlsx
+++ b/testData/Driver_Sanity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhinav.dagar\eclipse-workspace\platformOne\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA2CCE76-C11F-49EB-9303-A05F4D2E1362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430A39CA-81FE-4546-A70E-F363847E1FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{36864276-C195-4033-AAC0-6E76CEDE8C85}"/>
   </bookViews>
@@ -499,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD62453D-DA91-4664-9784-0086E4F2EC4E}">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -530,7 +530,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -538,7 +538,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -546,7 +546,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -554,7 +554,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -562,7 +562,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -570,7 +570,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -578,7 +578,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -586,7 +586,7 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -594,7 +594,7 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -610,7 +610,7 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -618,7 +618,7 @@
         <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -626,7 +626,7 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -634,7 +634,7 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -642,7 +642,7 @@
         <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -650,7 +650,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -658,7 +658,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -666,7 +666,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -674,7 +674,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -682,7 +682,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -690,7 +690,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -698,7 +698,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -706,7 +706,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -714,7 +714,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -722,7 +722,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
@@ -730,7 +730,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>